<commit_message>
DRILL-8417: Allow Excel Reader to Ignore Formula Errors
</commit_message>
<xml_diff>
--- a/contrib/format-excel/src/test/resources/excel/text-formula.xlsx
+++ b/contrib/format-excel/src/test/resources/excel/text-formula.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgivre/github/drill-dev/drill/contrib/format-excel/src/test/resources/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlesgivre/github/drill/contrib/format-excel/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DCE676-3DD9-2F43-8BCE-BF0A62D579B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24B4B2E-4569-8146-AE24-78101539A3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16000" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{9BCA75AE-1820-AD49-8302-CCB2DDF24DE2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="1" xr2:uid="{9BCA75AE-1820-AD49-8302-CCB2DDF24DE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet with Errors" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Seventh Grade</t>
   </si>
@@ -55,6 +56,15 @@
   </si>
   <si>
     <t>Combined</t>
+  </si>
+  <si>
+    <t>field2</t>
+  </si>
+  <si>
+    <t>field1</t>
+  </si>
+  <si>
+    <t>result</t>
   </si>
 </sst>
 </file>
@@ -415,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75247D58-FECF-0F48-BF94-67F107952465}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -474,4 +484,90 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD3BB08-43C1-F644-857A-C5E8932B64BA}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <f>A2/B2</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C6" si="0">A3/B3</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DRILL-8417: Allow Excel Reader to Ignore Formula Errors (#2783)
</commit_message>
<xml_diff>
--- a/contrib/format-excel/src/test/resources/excel/text-formula.xlsx
+++ b/contrib/format-excel/src/test/resources/excel/text-formula.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgivre/github/drill-dev/drill/contrib/format-excel/src/test/resources/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlesgivre/github/drill/contrib/format-excel/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DCE676-3DD9-2F43-8BCE-BF0A62D579B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24B4B2E-4569-8146-AE24-78101539A3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16000" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{9BCA75AE-1820-AD49-8302-CCB2DDF24DE2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="1" xr2:uid="{9BCA75AE-1820-AD49-8302-CCB2DDF24DE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet with Errors" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Seventh Grade</t>
   </si>
@@ -55,6 +56,15 @@
   </si>
   <si>
     <t>Combined</t>
+  </si>
+  <si>
+    <t>field2</t>
+  </si>
+  <si>
+    <t>field1</t>
+  </si>
+  <si>
+    <t>result</t>
   </si>
 </sst>
 </file>
@@ -415,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75247D58-FECF-0F48-BF94-67F107952465}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -474,4 +484,90 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD3BB08-43C1-F644-857A-C5E8932B64BA}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <f>A2/B2</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C6" si="0">A3/B3</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>